<commit_message>
MOVPE CNR schema design
</commit_message>
<xml_diff>
--- a/movpe_CNR/datafile.xlsx
+++ b/movpe_CNR/datafile.xlsx
@@ -137,7 +137,7 @@
     <t xml:space="preserve">Movpe sto</t>
   </si>
   <si>
-    <t xml:space="preserve">giorgio</t>
+    <t xml:space="preserve">5c87d4dd-5b6a-4759-9946-fff9bbd7cd44</t>
   </si>
   <si>
     <t xml:space="preserve">STO:La</t>
@@ -830,7 +830,7 @@
     <numFmt numFmtId="168" formatCode="0.00"/>
     <numFmt numFmtId="169" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -893,12 +893,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1228,7 +1222,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1331,8 +1325,8 @@
   </sheetPr>
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1352,7 +1346,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="39.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,7 +1516,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="R6" s="0"/>
+      <c r="R6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -4843,13 +4837,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="8.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.29"/>
@@ -5040,7 +5034,7 @@
         <v>233</v>
       </c>
       <c r="B6" s="56"/>
-      <c r="C6" s="0"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="57" t="n">
         <f aca="false">AVERAGE(D10:D12)</f>
         <v>736.666666666667</v>
@@ -5094,7 +5088,7 @@
         <v>235</v>
       </c>
       <c r="B7" s="56"/>
-      <c r="C7" s="0"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="57" t="n">
         <f aca="false">STDEVA(D10:D12)</f>
         <v>1.15470053837925</v>

</xml_diff>